<commit_message>
Add Aggregating data tutorial chapter
</commit_message>
<xml_diff>
--- a/docs/assets/data/music_data.xlsx
+++ b/docs/assets/data/music_data.xlsx
@@ -64,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,11 +86,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,7 +173,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -243,7 +246,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>36</v>

</xml_diff>